<commit_message>
finsih buit catalog builder
</commit_message>
<xml_diff>
--- a/tests/sample_tests_data/catalog/hypo_catalog.xlsx
+++ b/tests/sample_tests_data/catalog/hypo_catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SEML\GITHUB DEPLOY\LQTMomentMag\tests\sample_tests_data\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF93832-4712-42F1-86AB-B1170AA140C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F3DAF8-4820-4181-B4E1-A5899E16CCE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>t_0</t>
+  </si>
+  <si>
+    <t>remarks</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +514,9 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4">

</xml_diff>